<commit_message>
Cambio del campo hallazgo por finding
Se cambia el campo hallazgo por finding
Se agregan los campos date y time
Se actualiza el excel
</commit_message>
<xml_diff>
--- a/ecms/storage/app/public/campos_del_formulario.xlsx
+++ b/ecms/storage/app/public/campos_del_formulario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\paes\ecms\storage\app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22850DD-F9F9-4E84-8EAC-DEDB6E816A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40193C96-7EF3-4125-BA3F-D8D2269AC8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4330D20F-99AD-4B2E-8CE2-9831B312A000}"/>
   </bookViews>
@@ -148,7 +148,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Hallazgo:</t>
+          <t>Finding (Hallazgo):</t>
         </r>
         <r>
           <rPr>
@@ -231,7 +231,7 @@
     <t>Selectable</t>
   </si>
   <si>
-    <t>Hallazgo</t>
+    <t>Finding</t>
   </si>
 </sst>
 </file>
@@ -899,7 +899,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E17" sqref="E17:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,7 +931,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="aQP8uYdLMGgO7CSlgXiMx0pa0AbCiF24KQN5Bnxsq+8OHXDGVKsnQYTRbfHKlha96Q82j1elVXXtgs1VABMIXA==" saltValue="/PI6FDQ/MRYXD82HUCxs5g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="WHK1nB8BWHOFHTlNURnTE9N8eEBxWxTTGXvVb4aHlA9kH/65rccc0pyzfWIb4Iz9zNNSigVITSYsZRxASA1aZg==" saltValue="V6CzChOyo15eyHAZ1FqAHA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B2:B1425" xr:uid="{2A92CA4C-C7BC-4078-8F1D-2A416ADC822E}">
       <formula1>typeLabel</formula1>

</xml_diff>

<commit_message>
importacion de fecha y hora desde excel
</commit_message>
<xml_diff>
--- a/ecms/storage/app/public/campos_del_formulario.xlsx
+++ b/ecms/storage/app/public/campos_del_formulario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\paes\ecms\storage\app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40193C96-7EF3-4125-BA3F-D8D2269AC8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D48252-AB53-4B30-9837-51B76A861E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4330D20F-99AD-4B2E-8CE2-9831B312A000}"/>
   </bookViews>
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>type</t>
   </si>
@@ -232,6 +232,12 @@
   </si>
   <si>
     <t>Finding</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Hora</t>
   </si>
 </sst>
 </file>
@@ -580,8 +586,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ACC51220-2459-423B-B311-73EFA2644BC4}" name="Tabla1" displayName="Tabla1" ref="B2:B16" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="B2:B16" xr:uid="{ACC51220-2459-423B-B311-73EFA2644BC4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ACC51220-2459-423B-B311-73EFA2644BC4}" name="Tabla1" displayName="Tabla1" ref="B2:B18" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="B2:B18" xr:uid="{ACC51220-2459-423B-B311-73EFA2644BC4}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{7D15252D-1089-4EBD-913C-169F9BDBF46D}" name="type" dataDxfId="6"/>
   </tableColumns>
@@ -899,7 +905,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:E18"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,10 +963,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49B9D850-7A7D-4706-ACFB-17BDF3592C31}">
-  <dimension ref="B2:B16"/>
+  <dimension ref="B2:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,8 +1050,18 @@
         <v>9</v>
       </c>
     </row>
+    <row r="17" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="hPvQxQ0YtsFYJBXL5kTjIff0rTHbA/LldON+aTVK7Z+BiuFkLjlos3D6dJkkU5X7oWbmB9IdtRd1SbvNwr2z+g==" saltValue="XWRoL5BSpDeSLNDUZbQ6tA==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>